<commit_message>
all data is imported into the xlsx files, pdf files are individually exported and then combined. Final file is writen in "Site.final_output_dir" directory. Individual files are writen in "Site.output_dir" directory and then deleted
</commit_message>
<xml_diff>
--- a/checklistGenerator/xlsx/Antifoc.xlsx
+++ b/checklistGenerator/xlsx/Antifoc.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,32 +20,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
-  <si>
-    <t xml:space="preserve">În concordanță cu Contractul de service și mentenanță nr.: .....</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
+  <si>
+    <t xml:space="preserve">În concordanță cu Contractul de service și mentenanță nr.:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.....</t>
   </si>
   <si>
     <t xml:space="preserve">PRODUS:</t>
   </si>
   <si>
-    <t xml:space="preserve">USA ANTIFOC GLISANTA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Benficiar:</t>
   </si>
   <si>
-    <t xml:space="preserve">…..</t>
-  </si>
-  <si>
     <t xml:space="preserve">Locație:</t>
   </si>
   <si>
     <t xml:space="preserve">Anul fabricației: </t>
   </si>
   <si>
-    <t xml:space="preserve">.....</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comanda nr.:</t>
   </si>
   <si>
@@ -55,10 +49,10 @@
     <t xml:space="preserve">Dimensiuni (LxH):</t>
   </si>
   <si>
-    <t xml:space="preserve">.....x..... mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tel.:</t>
+    <t xml:space="preserve">.....x.....mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tel:</t>
   </si>
   <si>
     <t xml:space="preserve">0722 399 907</t>
@@ -73,7 +67,7 @@
     <t xml:space="preserve">www.da-te.ro</t>
   </si>
   <si>
-    <t xml:space="preserve">PRODUS: UȘĂ ANTIFOC GLISANTĂ CU (UN CANAT/ DOUĂ CANATE)</t>
+    <t xml:space="preserve">PRODUS: .....</t>
   </si>
   <si>
     <t xml:space="preserve">Nr.</t>
@@ -89,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nr. bucăți</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cod articol</t>
   </si>
   <si>
     <t xml:space="preserve">Observații</t>
@@ -298,7 +289,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -359,24 +350,20 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -406,9 +393,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2417040</xdr:colOff>
+      <xdr:colOff>203400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -421,12 +408,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5670000" y="0"/>
-          <a:ext cx="2853360" cy="1252440"/>
+          <a:off x="5819040" y="0"/>
+          <a:ext cx="2850840" cy="1250640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
         </a:ln>
@@ -437,144 +425,318 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1f497d"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="eeece1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4f81bd"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="c0504d"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9bbb59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064a2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4bacc6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="f79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ff"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H58"/>
+  <dimension ref="B1:G58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="41.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="37.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G10" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H10" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -582,446 +744,418 @@
         <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="10" t="n">
         <v>3</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="10" t="n">
         <v>4</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="10" t="n">
         <v>5</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="10" t="n">
         <v>6</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="10" t="n">
         <v>7</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="10" t="n">
         <v>8</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="10" t="n">
         <v>9</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="10" t="n">
         <v>10</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="10" t="n">
         <v>11</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="10" t="n">
         <v>12</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="10" t="n">
         <v>13</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="10" t="n">
         <v>14</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="10" t="n">
         <v>15</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
       <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="10" t="n">
         <v>16</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="10" t="n">
         <v>17</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="10" t="n">
         <v>18</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
       <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="10" t="n">
         <v>19</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
       <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="10" t="n">
         <v>20</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
       <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="10" t="n">
         <v>21</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
       <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="10" t="n">
         <v>22</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
       <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="10" t="n">
         <v>23</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
       <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="10" t="n">
         <v>24</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
       <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="10" t="n">
         <v>25</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
       <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-    </row>
-    <row r="39" customFormat="false" ht="26.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="39" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="10" t="n">
         <v>26</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
       <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="15"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-    </row>
-    <row r="47" customFormat="false" ht="18.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-    </row>
-    <row r="48" customFormat="false" ht="18.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+    </row>
+    <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C49" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C50" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C51" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1031,7 +1165,6 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="4"/>
@@ -1040,7 +1173,6 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="4"/>
@@ -1049,18 +1181,17 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="57" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="18.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="57" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C47:G47"/>
     <mergeCell ref="C48:F48"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H10" r:id="rId1" display="www.da-te.ro"/>
+    <hyperlink ref="G10" r:id="rId1" display="www.da-te.ro"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.6" bottom="0.6" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>